<commit_message>
Added social links and logic
</commit_message>
<xml_diff>
--- a/newyear2018.xlsx
+++ b/newyear2018.xlsx
@@ -30,7 +30,7 @@
     <t>Profile</t>
   </si>
   <si>
-    <t>Quand vous recevez un devis</t>
+    <t>Quand vous recevez un devis :</t>
   </si>
   <si>
     <t>Vous vous précipitez sur le total, tout en bas de la page.</t>
@@ -99,7 +99,7 @@
     <t>Une souffrance.</t>
   </si>
   <si>
-    <t>Pour vous, un logo réussi c’est</t>
+    <t>Pour vous, un logo réussi c’est :</t>
   </si>
   <si>
     <t>Un peu comme un pull over : chaud, coloré et qui ne pique pas trop.</t>
@@ -114,10 +114,10 @@
     <t>Un joli dégradé, une ombre portée et un animal très mignon.</t>
   </si>
   <si>
-    <t>Toujours celui proposé par l’agence, piste n°1</t>
+    <t>Toujours celui proposé par l’agence, piste n°1.</t>
   </si>
   <si>
-    <t>Parmi ces délais, lesquels jugez vous «acceptables»</t>
+    <t>Parmi ces délais, lesquels jugez vous «acceptables» :</t>
   </si>
   <si>
     <t>Un site responsive en 1 semaine.</t>
@@ -138,7 +138,7 @@
     <t>Ceux proposés par l’agence, toujours.</t>
   </si>
   <si>
-    <t>Quand on vous dit «Dézipper», ça vous évoque</t>
+    <t>Quand on vous dit «Dézipper», ça vous évoque :</t>
   </si>
   <si>
     <t>Un truc en rapport avec vos mails mais que vous n’avez jamais réussi à maîtriser.</t>
@@ -150,10 +150,10 @@
     <t>Du lourd, du très lourd.</t>
   </si>
   <si>
-    <t>Euh, vous voulez dire «unzip», no?</t>
+    <t>Euh, vous voulez dire « unzip », no?</t>
   </si>
   <si>
-    <t>Pour nous envoyer vos corrections</t>
+    <t>Pour nous envoyer vos corrections :</t>
   </si>
   <si>
     <t>Vous privilégiez la formule : crayon de papier HB + sortie papier A3 + scan = pièce jointe de 2,3 Go.</t>
@@ -171,7 +171,7 @@
     <t>Une correction typo = un email, vous trouvez ça plus simple.</t>
   </si>
   <si>
-    <t>Un déjeuner avec nous c’est</t>
+    <t>Un déjeuner avec nous c’est :</t>
   </si>
   <si>
     <t>Un moment un peu gênant…</t>
@@ -207,7 +207,7 @@
     <t>Des communicants mais aussi des imprimeurs, des décorateurs d’intérieur, des journalistes, des poseurs de palissade… bref un peu tout ce dont vous avez besoin.</t>
   </si>
   <si>
-    <t>Votre radio préférée</t>
+    <t>Votre radio préférée :</t>
   </si>
   <si>
     <t>France culture, dès 6h le matin. Vous ne ratez jamais un podcast.</t>
@@ -228,28 +228,28 @@
     <t>Aucune. Vous zappez souvent.</t>
   </si>
   <si>
-    <t>Votre moyen de communication préféré</t>
+    <t>Votre moyen de communication préféré :</t>
   </si>
   <si>
-    <t>Snapchat</t>
+    <t>Snapchat.</t>
   </si>
   <si>
-    <t>Le fax</t>
+    <t>Le fax.</t>
   </si>
   <si>
-    <t>L’email</t>
+    <t>L’email.</t>
   </si>
   <si>
-    <t>Le téléphone</t>
+    <t>Le téléphone.</t>
   </si>
   <si>
-    <t>La réunion</t>
+    <t>La réunion.</t>
   </si>
   <si>
-    <t>Une bonne gueulante, ça réveille les troupes</t>
+    <t>Une bonne gueulante, ça réveille les troupes.</t>
   </si>
   <si>
-    <t>Votre animal totem</t>
+    <t>Votre animal totem :</t>
   </si>
   <si>
     <t>Le pangolin, trop stylé…</t>
@@ -267,22 +267,22 @@
     <t>Le lamantin, trop doux…</t>
   </si>
   <si>
-    <t>Vous êtes invité à un goûter d’anniversaire, vous vous jetez sur</t>
+    <t>Vous êtes invité à un goûter d’anniversaire, vous vous jetez sur :</t>
   </si>
   <si>
-    <t>Les « raider »</t>
+    <t>Les « raider ».</t>
   </si>
   <si>
-    <t>Les oursons en guimauve</t>
+    <t>Les oursons en guimauve.</t>
   </si>
   <si>
-    <t>Les couilles de mammouth</t>
+    <t>Les couilles de mammouth.</t>
   </si>
   <si>
-    <t>Les langues bien acides</t>
+    <t>Les langues bien acides.</t>
   </si>
   <si>
-    <t>Le champagne</t>
+    <t>Le champagne.</t>
   </si>
   <si>
     <t>A</t>
@@ -569,10 +569,10 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
@@ -601,10 +601,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -616,10 +616,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -637,13 +637,13 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -661,13 +661,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -826,13 +826,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -931,10 +925,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1189,13 +1183,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1508,10 +1496,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1800,19 +1788,19 @@
   </cols>
   <sheetData>
     <row r="1" ht="24.65" customHeight="1">
-      <c r="A1" t="s" s="3">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
       <c r="F1" s="4"/>
@@ -28341,32 +28329,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B46:B51"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="A58:A62"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A63:A67"/>
     <mergeCell ref="B63:B67"/>
     <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B46:B51"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B2:B6"/>
     <mergeCell ref="A52:A57"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="A58:A62"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A41:A45"/>
     <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B52:B57"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Update texts before launching
</commit_message>
<xml_diff>
--- a/newyear2018.xlsx
+++ b/newyear2018.xlsx
@@ -39,7 +39,7 @@
     <t>Cost-killer</t>
   </si>
   <si>
-    <t>Vous vérifiez qu’il prévoit un nombre illimité d’aller-retours créa.</t>
+    <t>Vous vérifiez qu’il prévoit un nombre illimité d’allers-retours créa.</t>
   </si>
   <si>
     <t>Angoissé du brief</t>
@@ -54,7 +54,7 @@
     <t>Pas besoin de le lire, c’est forcément trop cher : faites un effort !</t>
   </si>
   <si>
-    <t>Parler d’argent, c’est vulgaire non ?</t>
+    <t>Parler d’argent, c’est vulgaire, non ?</t>
   </si>
   <si>
     <t>BFF (best friend forever)</t>
@@ -84,7 +84,7 @@
     <t>Rien du tout.</t>
   </si>
   <si>
-    <t>Ecrire un brief, c’est :</t>
+    <t>Écrire un brief, c’est :</t>
   </si>
   <si>
     <t>Votre petit plaisir solitaire du vendredi soir.</t>
@@ -93,7 +93,7 @@
     <t>Toujours très concis : 3 lignes et pis zou !</t>
   </si>
   <si>
-    <t>Toujours ultra détaillé : 8 pages minimum, 5 réunions de pré-brief, 7 call et 3 aller-retour de validation avec votre boss.</t>
+    <t>Toujours ultra détaillé : 8 pages minimum, 5 réunions de pré-brief, 7 calls et 3 allers-retours de validation avec votre boss.</t>
   </si>
   <si>
     <t>Une souffrance.</t>
@@ -102,7 +102,7 @@
     <t>Pour vous, un logo réussi c’est :</t>
   </si>
   <si>
-    <t>Un peu comme un pull over : chaud, coloré et qui ne pique pas trop.</t>
+    <t>Un peu comme un pull-over : chaud, coloré et qui ne pique pas trop.</t>
   </si>
   <si>
     <t>Celui que vous avez déjà dessiné.</t>
@@ -114,10 +114,10 @@
     <t>Un joli dégradé, une ombre portée et un animal très mignon.</t>
   </si>
   <si>
-    <t>Toujours celui proposé par l’agence, piste n°1.</t>
+    <t>Toujours celui proposé par l’agence, piste n° 1.</t>
   </si>
   <si>
-    <t>Parmi ces délais, lesquels jugez vous «acceptables» :</t>
+    <t>Parmi ces délais, lesquels jugez-vous «acceptables» :</t>
   </si>
   <si>
     <t>Un site responsive en 1 semaine.</t>
@@ -126,7 +126,7 @@
     <t>Une carte de vœux en 2 heures.</t>
   </si>
   <si>
-    <t>Un plan de communication tri annuel en 15 jours.</t>
+    <t>Un plan de communication triannuel en 15 jours.</t>
   </si>
   <si>
     <t>6 mois entre deux réunions.</t>
@@ -138,10 +138,10 @@
     <t>Ceux proposés par l’agence, toujours.</t>
   </si>
   <si>
-    <t>Quand on vous dit «Dézipper», ça vous évoque :</t>
+    <t>Quand on vous dit «dézipper», ça vous évoque :</t>
   </si>
   <si>
-    <t>Un truc en rapport avec vos mails mais que vous n’avez jamais réussi à maîtriser.</t>
+    <t>Un truc en rapport avec vos e-mails mais que vous n’avez jamais réussi à maîtriser.</t>
   </si>
   <si>
     <t>Le bois de Boulogne.</t>
@@ -150,7 +150,7 @@
     <t>Du lourd, du très lourd.</t>
   </si>
   <si>
-    <t>Euh, vous voulez dire « unzip », no?</t>
+    <t>Euh, vous voulez dire « unzip », no ?</t>
   </si>
   <si>
     <t>Pour nous envoyer vos corrections :</t>
@@ -168,16 +168,16 @@
     <t>Vous nous faites une confiance aveugle.</t>
   </si>
   <si>
-    <t>Une correction typo = un email, vous trouvez ça plus simple.</t>
+    <t>Une correction typo = un e-mail, vous trouvez ça plus simple.</t>
   </si>
   <si>
-    <t>Un déjeuner avec nous c’est :</t>
+    <t>Un déjeuner avec nous, c’est :</t>
   </si>
   <si>
     <t>Un moment un peu gênant…</t>
   </si>
   <si>
-    <t>Un ticket resto économisé.</t>
+    <t>Un ticket-resto économisé.</t>
   </si>
   <si>
     <t>Toujours en soirée, pour pouvoir picoler.</t>
@@ -189,7 +189,7 @@
     <t>Vous qui invitez !</t>
   </si>
   <si>
-    <t>Quand vous pensez à une agence de com’… Vous imaginez d’abord :</t>
+    <t>Quand vous pensez à une agence de com… Vous imaginez d’abord :</t>
   </si>
   <si>
     <t>Une bande de graphistes + un mec qui réfléchit.</t>
@@ -204,19 +204,19 @@
     <t>Vos meilleurs alliés.</t>
   </si>
   <si>
-    <t>Des communicants mais aussi des imprimeurs, des décorateurs d’intérieur, des journalistes, des poseurs de palissade… bref un peu tout ce dont vous avez besoin.</t>
+    <t>Des communicants mais aussi des imprimeurs, des décorateurs d’intérieur, des journalistes, des poseurs de palissades… bref un peu tout ce dont vous avez besoin.</t>
   </si>
   <si>
     <t>Votre radio préférée :</t>
   </si>
   <si>
-    <t>France culture, dès 6h le matin. Vous ne ratez jamais un podcast.</t>
+    <t>France Culture, dès 6 h le matin. Vous ne ratez jamais un podcast.</t>
   </si>
   <si>
     <t>Nostalgie, vous n’écoutez que du Sardou.</t>
   </si>
   <si>
-    <t>Nova, entre 2h et 5h du mat’, en rentrant de soirée.</t>
+    <t>Nova, entre 2 h et 5 h du mat, en rentrant de soirée.</t>
   </si>
   <si>
     <t>BFM, l’éco avant tout.</t>
@@ -237,7 +237,7 @@
     <t>Le fax.</t>
   </si>
   <si>
-    <t>L’email.</t>
+    <t>L’e-mail.</t>
   </si>
   <si>
     <t>Le téléphone.</t>
@@ -255,7 +255,7 @@
     <t>Le pangolin, trop stylé…</t>
   </si>
   <si>
-    <t>La tarsier, trop choupinou…</t>
+    <t>Le tarsier, trop choupinou…</t>
   </si>
   <si>
     <t>Le concombre de mer, trop alternatif…</t>
@@ -267,7 +267,7 @@
     <t>Le lamantin, trop doux…</t>
   </si>
   <si>
-    <t>Vous êtes invité à un goûter d’anniversaire, vous vous jetez sur :</t>
+    <t>Vous êtes invité-e à un goûter d’anniversaire, vous vous jetez sur :</t>
   </si>
   <si>
     <t>Les « raider ».</t>
@@ -28329,32 +28329,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B52:B57"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B46:B51"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B58:B62"/>
     <mergeCell ref="A58:A62"/>
     <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B31:B35"/>
     <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="B63:B67"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B46:B51"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A52:A57"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B52:B57"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="A2:A6"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>